<commit_message>
Parallax Background + fixed resolution bug + anti aliasing
</commit_message>
<xml_diff>
--- a/Design/problems.xlsx
+++ b/Design/problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l\Desktop\desktop\programming\Unity\Shooter\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B2DB43-F083-4B35-9DB5-C1CE91D7D076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC88DDD0-2670-4836-8D3F-8B99B144CCC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12682" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>check</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -143,6 +143,10 @@
   </si>
   <si>
     <t>首先原素材要足够高清。其次分辨率不能过低也不能过高（超过原图清晰度也会有锯齿）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分辨率变高后worldToScreen返回的屏幕坐标就变大了，但UI中的坐标尺度却没有变化</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -197,10 +201,10 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -485,7 +489,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.95" x14ac:dyDescent="0.25"/>
@@ -608,6 +612,9 @@
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="E7" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">

</xml_diff>

<commit_message>
bullet polish: reflection & fade out
</commit_message>
<xml_diff>
--- a/Design/problems.xlsx
+++ b/Design/problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l\Desktop\desktop\programming\Unity\Shooter\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC88DDD0-2670-4836-8D3F-8B99B144CCC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1679A0C1-2ADE-4A1E-B326-1150EB47D297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12682" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>check</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -147,6 +147,10 @@
   </si>
   <si>
     <t>分辨率变高后worldToScreen返回的屏幕坐标就变大了，但UI中的坐标尺度却没有变化</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冲刺后后坐力驱动bug</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -486,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.95" x14ac:dyDescent="0.25"/>
@@ -630,6 +634,17 @@
         <v>21</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New feature: Camera Deadzone
</commit_message>
<xml_diff>
--- a/Design/problems.xlsx
+++ b/Design/problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l\Desktop\desktop\programming\Unity\Shooter\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1679A0C1-2ADE-4A1E-B326-1150EB47D297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9D9DEC-4B4B-4181-BEA4-9C05D620D84C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12682" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>check</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -147,10 +147,6 @@
   </si>
   <si>
     <t>分辨率变高后worldToScreen返回的屏幕坐标就变大了，但UI中的坐标尺度却没有变化</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>冲刺后后坐力驱动bug</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -493,7 +489,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.95" x14ac:dyDescent="0.25"/>
@@ -638,12 +634,6 @@
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>